<commit_message>
Populate price variation data and add to price docs.
</commit_message>
<xml_diff>
--- a/PriceScenarios.xlsx
+++ b/PriceScenarios.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="14">
   <si>
     <t>typ</t>
   </si>
@@ -50,6 +50,15 @@
   </si>
   <si>
     <t>c1_0</t>
+  </si>
+  <si>
+    <t>c1_1</t>
+  </si>
+  <si>
+    <t>c1_2</t>
+  </si>
+  <si>
+    <t>c1_3</t>
   </si>
 </sst>
 </file>
@@ -407,7 +416,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -450,34 +459,139 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0.8517948448018292</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0.8517948448018292</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0.8517948448018292</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0.8517948448018292</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0.8517948448018292</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0.8517948448018292</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0.8517948448018292</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0.8517948448018292</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>0.8517948448018292</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>0.8517948448018292</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>0.8475773720402696</v>
+      </c>
+      <c r="C3">
+        <v>0.8475773720402696</v>
+      </c>
+      <c r="D3">
+        <v>0.8475773720402696</v>
+      </c>
+      <c r="E3">
+        <v>0.8475773720402696</v>
+      </c>
+      <c r="F3">
+        <v>0.8475773720402696</v>
+      </c>
+      <c r="G3">
+        <v>0.8475773720402696</v>
+      </c>
+      <c r="H3">
+        <v>0.8475773720402696</v>
+      </c>
+      <c r="I3">
+        <v>0.8475773720402696</v>
+      </c>
+      <c r="J3">
+        <v>0.8475773720402696</v>
+      </c>
+      <c r="K3">
+        <v>0.8475773720402696</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>1.153146674367855</v>
+      </c>
+      <c r="C4">
+        <v>1.153146674367855</v>
+      </c>
+      <c r="D4">
+        <v>1.153146674367855</v>
+      </c>
+      <c r="E4">
+        <v>1.153146674367855</v>
+      </c>
+      <c r="F4">
+        <v>1.153146674367855</v>
+      </c>
+      <c r="G4">
+        <v>1.153146674367855</v>
+      </c>
+      <c r="H4">
+        <v>1.153146674367855</v>
+      </c>
+      <c r="I4">
+        <v>1.153146674367855</v>
+      </c>
+      <c r="J4">
+        <v>1.153146674367855</v>
+      </c>
+      <c r="K4">
+        <v>1.153146674367855</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>1.147437125033402</v>
+      </c>
+      <c r="C5">
+        <v>1.147437125033402</v>
+      </c>
+      <c r="D5">
+        <v>1.147437125033402</v>
+      </c>
+      <c r="E5">
+        <v>1.147437125033402</v>
+      </c>
+      <c r="F5">
+        <v>1.147437125033402</v>
+      </c>
+      <c r="G5">
+        <v>1.147437125033402</v>
+      </c>
+      <c r="H5">
+        <v>1.147437125033402</v>
+      </c>
+      <c r="I5">
+        <v>1.147437125033402</v>
+      </c>
+      <c r="J5">
+        <v>1.147437125033402</v>
+      </c>
+      <c r="K5">
+        <v>1.147437125033402</v>
       </c>
     </row>
   </sheetData>
@@ -487,7 +601,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -530,34 +644,139 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0.706002939353065</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0.706002939353065</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0.706002939353065</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0.706002939353065</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0.706002939353065</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0.706002939353065</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0.706002939353065</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0.706002939353065</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>0.706002939353065</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>0.706002939353065</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>1.303792821776162</v>
+      </c>
+      <c r="C3">
+        <v>1.303792821776162</v>
+      </c>
+      <c r="D3">
+        <v>1.303792821776162</v>
+      </c>
+      <c r="E3">
+        <v>1.303792821776162</v>
+      </c>
+      <c r="F3">
+        <v>1.303792821776162</v>
+      </c>
+      <c r="G3">
+        <v>1.303792821776162</v>
+      </c>
+      <c r="H3">
+        <v>1.303792821776162</v>
+      </c>
+      <c r="I3">
+        <v>1.303792821776162</v>
+      </c>
+      <c r="J3">
+        <v>1.303792821776162</v>
+      </c>
+      <c r="K3">
+        <v>1.303792821776162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>0.6962071782238374</v>
+      </c>
+      <c r="C4">
+        <v>0.6962071782238374</v>
+      </c>
+      <c r="D4">
+        <v>0.6962071782238374</v>
+      </c>
+      <c r="E4">
+        <v>0.6962071782238374</v>
+      </c>
+      <c r="F4">
+        <v>0.6962071782238374</v>
+      </c>
+      <c r="G4">
+        <v>0.6962071782238374</v>
+      </c>
+      <c r="H4">
+        <v>0.6962071782238374</v>
+      </c>
+      <c r="I4">
+        <v>0.6962071782238374</v>
+      </c>
+      <c r="J4">
+        <v>0.6962071782238374</v>
+      </c>
+      <c r="K4">
+        <v>0.6962071782238374</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>1.293997060646935</v>
+      </c>
+      <c r="C5">
+        <v>1.293997060646935</v>
+      </c>
+      <c r="D5">
+        <v>1.293997060646935</v>
+      </c>
+      <c r="E5">
+        <v>1.293997060646935</v>
+      </c>
+      <c r="F5">
+        <v>1.293997060646935</v>
+      </c>
+      <c r="G5">
+        <v>1.293997060646935</v>
+      </c>
+      <c r="H5">
+        <v>1.293997060646935</v>
+      </c>
+      <c r="I5">
+        <v>1.293997060646935</v>
+      </c>
+      <c r="J5">
+        <v>1.293997060646935</v>
+      </c>
+      <c r="K5">
+        <v>1.293997060646935</v>
       </c>
     </row>
   </sheetData>
@@ -567,7 +786,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -610,34 +829,139 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0.706002939353065</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0.706002939353065</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0.706002939353065</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0.706002939353065</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0.706002939353065</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0.706002939353065</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0.706002939353065</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0.706002939353065</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>0.706002939353065</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>0.706002939353065</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>1.303792821776162</v>
+      </c>
+      <c r="C3">
+        <v>1.303792821776162</v>
+      </c>
+      <c r="D3">
+        <v>1.303792821776162</v>
+      </c>
+      <c r="E3">
+        <v>1.303792821776162</v>
+      </c>
+      <c r="F3">
+        <v>1.303792821776162</v>
+      </c>
+      <c r="G3">
+        <v>1.303792821776162</v>
+      </c>
+      <c r="H3">
+        <v>1.303792821776162</v>
+      </c>
+      <c r="I3">
+        <v>1.303792821776162</v>
+      </c>
+      <c r="J3">
+        <v>1.303792821776162</v>
+      </c>
+      <c r="K3">
+        <v>1.303792821776162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>0.6962071782238374</v>
+      </c>
+      <c r="C4">
+        <v>0.6962071782238374</v>
+      </c>
+      <c r="D4">
+        <v>0.6962071782238374</v>
+      </c>
+      <c r="E4">
+        <v>0.6962071782238374</v>
+      </c>
+      <c r="F4">
+        <v>0.6962071782238374</v>
+      </c>
+      <c r="G4">
+        <v>0.6962071782238374</v>
+      </c>
+      <c r="H4">
+        <v>0.6962071782238374</v>
+      </c>
+      <c r="I4">
+        <v>0.6962071782238374</v>
+      </c>
+      <c r="J4">
+        <v>0.6962071782238374</v>
+      </c>
+      <c r="K4">
+        <v>0.6962071782238374</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>1.293997060646935</v>
+      </c>
+      <c r="C5">
+        <v>1.293997060646935</v>
+      </c>
+      <c r="D5">
+        <v>1.293997060646935</v>
+      </c>
+      <c r="E5">
+        <v>1.293997060646935</v>
+      </c>
+      <c r="F5">
+        <v>1.293997060646935</v>
+      </c>
+      <c r="G5">
+        <v>1.293997060646935</v>
+      </c>
+      <c r="H5">
+        <v>1.293997060646935</v>
+      </c>
+      <c r="I5">
+        <v>1.293997060646935</v>
+      </c>
+      <c r="J5">
+        <v>1.293997060646935</v>
+      </c>
+      <c r="K5">
+        <v>1.293997060646935</v>
       </c>
     </row>
   </sheetData>
@@ -647,7 +971,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -663,7 +987,31 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0.2426304458088387</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>0.2573695541911614</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>0.2573695541911612</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>0.2426304458088387</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add second method to price scenario generation - moving average to de-trend data.
</commit_message>
<xml_diff>
--- a/PriceScenarios.xlsx
+++ b/PriceScenarios.xlsx
@@ -459,34 +459,34 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>0.8517948448018292</v>
+        <v>0.9001469258456177</v>
       </c>
       <c r="C2">
-        <v>0.8517948448018292</v>
+        <v>0.9001469258456177</v>
       </c>
       <c r="D2">
-        <v>0.8517948448018292</v>
+        <v>0.9001469258456177</v>
       </c>
       <c r="E2">
-        <v>0.8517948448018292</v>
+        <v>0.9001469258456177</v>
       </c>
       <c r="F2">
-        <v>0.8517948448018292</v>
+        <v>0.9001469258456177</v>
       </c>
       <c r="G2">
-        <v>0.8517948448018292</v>
+        <v>0.9001469258456177</v>
       </c>
       <c r="H2">
-        <v>0.8517948448018292</v>
+        <v>0.9001469258456177</v>
       </c>
       <c r="I2">
-        <v>0.8517948448018292</v>
+        <v>0.9001469258456177</v>
       </c>
       <c r="J2">
-        <v>0.8517948448018292</v>
+        <v>0.9001469258456177</v>
       </c>
       <c r="K2">
-        <v>0.8517948448018292</v>
+        <v>0.9001469258456177</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -494,34 +494,34 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>0.8475773720402696</v>
+        <v>0.8759941262449619</v>
       </c>
       <c r="C3">
-        <v>0.8475773720402696</v>
+        <v>0.8759941262449619</v>
       </c>
       <c r="D3">
-        <v>0.8475773720402696</v>
+        <v>0.8759941262449619</v>
       </c>
       <c r="E3">
-        <v>0.8475773720402696</v>
+        <v>0.8759941262449619</v>
       </c>
       <c r="F3">
-        <v>0.8475773720402696</v>
+        <v>0.8759941262449619</v>
       </c>
       <c r="G3">
-        <v>0.8475773720402696</v>
+        <v>0.8759941262449619</v>
       </c>
       <c r="H3">
-        <v>0.8475773720402696</v>
+        <v>0.8759941262449619</v>
       </c>
       <c r="I3">
-        <v>0.8475773720402696</v>
+        <v>0.8759941262449619</v>
       </c>
       <c r="J3">
-        <v>0.8475773720402696</v>
+        <v>0.8759941262449619</v>
       </c>
       <c r="K3">
-        <v>0.8475773720402696</v>
+        <v>0.8759941262449619</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -529,34 +529,34 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>1.153146674367855</v>
+        <v>1.124005873755038</v>
       </c>
       <c r="C4">
-        <v>1.153146674367855</v>
+        <v>1.124005873755038</v>
       </c>
       <c r="D4">
-        <v>1.153146674367855</v>
+        <v>1.124005873755038</v>
       </c>
       <c r="E4">
-        <v>1.153146674367855</v>
+        <v>1.124005873755038</v>
       </c>
       <c r="F4">
-        <v>1.153146674367855</v>
+        <v>1.124005873755038</v>
       </c>
       <c r="G4">
-        <v>1.153146674367855</v>
+        <v>1.124005873755038</v>
       </c>
       <c r="H4">
-        <v>1.153146674367855</v>
+        <v>1.124005873755038</v>
       </c>
       <c r="I4">
-        <v>1.153146674367855</v>
+        <v>1.124005873755038</v>
       </c>
       <c r="J4">
-        <v>1.153146674367855</v>
+        <v>1.124005873755038</v>
       </c>
       <c r="K4">
-        <v>1.153146674367855</v>
+        <v>1.124005873755038</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -564,34 +564,34 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>1.147437125033402</v>
+        <v>1.099853074154382</v>
       </c>
       <c r="C5">
-        <v>1.147437125033402</v>
+        <v>1.099853074154382</v>
       </c>
       <c r="D5">
-        <v>1.147437125033402</v>
+        <v>1.099853074154382</v>
       </c>
       <c r="E5">
-        <v>1.147437125033402</v>
+        <v>1.099853074154382</v>
       </c>
       <c r="F5">
-        <v>1.147437125033402</v>
+        <v>1.099853074154382</v>
       </c>
       <c r="G5">
-        <v>1.147437125033402</v>
+        <v>1.099853074154382</v>
       </c>
       <c r="H5">
-        <v>1.147437125033402</v>
+        <v>1.099853074154382</v>
       </c>
       <c r="I5">
-        <v>1.147437125033402</v>
+        <v>1.099853074154382</v>
       </c>
       <c r="J5">
-        <v>1.147437125033402</v>
+        <v>1.099853074154382</v>
       </c>
       <c r="K5">
-        <v>1.147437125033402</v>
+        <v>1.099853074154382</v>
       </c>
     </row>
   </sheetData>
@@ -644,34 +644,34 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>0.706002939353065</v>
+        <v>0.8167959426209745</v>
       </c>
       <c r="C2">
-        <v>0.706002939353065</v>
+        <v>0.8167959426209745</v>
       </c>
       <c r="D2">
-        <v>0.706002939353065</v>
+        <v>0.8167959426209745</v>
       </c>
       <c r="E2">
-        <v>0.706002939353065</v>
+        <v>0.8167959426209745</v>
       </c>
       <c r="F2">
-        <v>0.706002939353065</v>
+        <v>0.8167959426209745</v>
       </c>
       <c r="G2">
-        <v>0.706002939353065</v>
+        <v>0.8167959426209745</v>
       </c>
       <c r="H2">
-        <v>0.706002939353065</v>
+        <v>0.8167959426209745</v>
       </c>
       <c r="I2">
-        <v>0.706002939353065</v>
+        <v>0.8167959426209745</v>
       </c>
       <c r="J2">
-        <v>0.706002939353065</v>
+        <v>0.8167959426209745</v>
       </c>
       <c r="K2">
-        <v>0.706002939353065</v>
+        <v>0.8167959426209745</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -679,34 +679,34 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>1.303792821776162</v>
+        <v>1.227518074963115</v>
       </c>
       <c r="C3">
-        <v>1.303792821776162</v>
+        <v>1.227518074963115</v>
       </c>
       <c r="D3">
-        <v>1.303792821776162</v>
+        <v>1.227518074963115</v>
       </c>
       <c r="E3">
-        <v>1.303792821776162</v>
+        <v>1.227518074963115</v>
       </c>
       <c r="F3">
-        <v>1.303792821776162</v>
+        <v>1.227518074963115</v>
       </c>
       <c r="G3">
-        <v>1.303792821776162</v>
+        <v>1.227518074963115</v>
       </c>
       <c r="H3">
-        <v>1.303792821776162</v>
+        <v>1.227518074963115</v>
       </c>
       <c r="I3">
-        <v>1.303792821776162</v>
+        <v>1.227518074963115</v>
       </c>
       <c r="J3">
-        <v>1.303792821776162</v>
+        <v>1.227518074963115</v>
       </c>
       <c r="K3">
-        <v>1.303792821776162</v>
+        <v>1.227518074963115</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -714,34 +714,34 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>0.6962071782238374</v>
+        <v>0.7724819250368852</v>
       </c>
       <c r="C4">
-        <v>0.6962071782238374</v>
+        <v>0.7724819250368852</v>
       </c>
       <c r="D4">
-        <v>0.6962071782238374</v>
+        <v>0.7724819250368852</v>
       </c>
       <c r="E4">
-        <v>0.6962071782238374</v>
+        <v>0.7724819250368852</v>
       </c>
       <c r="F4">
-        <v>0.6962071782238374</v>
+        <v>0.7724819250368852</v>
       </c>
       <c r="G4">
-        <v>0.6962071782238374</v>
+        <v>0.7724819250368852</v>
       </c>
       <c r="H4">
-        <v>0.6962071782238374</v>
+        <v>0.7724819250368852</v>
       </c>
       <c r="I4">
-        <v>0.6962071782238374</v>
+        <v>0.7724819250368852</v>
       </c>
       <c r="J4">
-        <v>0.6962071782238374</v>
+        <v>0.7724819250368852</v>
       </c>
       <c r="K4">
-        <v>0.6962071782238374</v>
+        <v>0.7724819250368852</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -749,34 +749,34 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>1.293997060646935</v>
+        <v>1.183204057379025</v>
       </c>
       <c r="C5">
-        <v>1.293997060646935</v>
+        <v>1.183204057379025</v>
       </c>
       <c r="D5">
-        <v>1.293997060646935</v>
+        <v>1.183204057379025</v>
       </c>
       <c r="E5">
-        <v>1.293997060646935</v>
+        <v>1.183204057379025</v>
       </c>
       <c r="F5">
-        <v>1.293997060646935</v>
+        <v>1.183204057379025</v>
       </c>
       <c r="G5">
-        <v>1.293997060646935</v>
+        <v>1.183204057379025</v>
       </c>
       <c r="H5">
-        <v>1.293997060646935</v>
+        <v>1.183204057379025</v>
       </c>
       <c r="I5">
-        <v>1.293997060646935</v>
+        <v>1.183204057379025</v>
       </c>
       <c r="J5">
-        <v>1.293997060646935</v>
+        <v>1.183204057379025</v>
       </c>
       <c r="K5">
-        <v>1.293997060646935</v>
+        <v>1.183204057379025</v>
       </c>
     </row>
   </sheetData>
@@ -829,34 +829,34 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>0.706002939353065</v>
+        <v>0.8167959426209745</v>
       </c>
       <c r="C2">
-        <v>0.706002939353065</v>
+        <v>0.8167959426209745</v>
       </c>
       <c r="D2">
-        <v>0.706002939353065</v>
+        <v>0.8167959426209745</v>
       </c>
       <c r="E2">
-        <v>0.706002939353065</v>
+        <v>0.8167959426209745</v>
       </c>
       <c r="F2">
-        <v>0.706002939353065</v>
+        <v>0.8167959426209745</v>
       </c>
       <c r="G2">
-        <v>0.706002939353065</v>
+        <v>0.8167959426209745</v>
       </c>
       <c r="H2">
-        <v>0.706002939353065</v>
+        <v>0.8167959426209745</v>
       </c>
       <c r="I2">
-        <v>0.706002939353065</v>
+        <v>0.8167959426209745</v>
       </c>
       <c r="J2">
-        <v>0.706002939353065</v>
+        <v>0.8167959426209745</v>
       </c>
       <c r="K2">
-        <v>0.706002939353065</v>
+        <v>0.8167959426209745</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -864,34 +864,34 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>1.303792821776162</v>
+        <v>1.227518074963115</v>
       </c>
       <c r="C3">
-        <v>1.303792821776162</v>
+        <v>1.227518074963115</v>
       </c>
       <c r="D3">
-        <v>1.303792821776162</v>
+        <v>1.227518074963115</v>
       </c>
       <c r="E3">
-        <v>1.303792821776162</v>
+        <v>1.227518074963115</v>
       </c>
       <c r="F3">
-        <v>1.303792821776162</v>
+        <v>1.227518074963115</v>
       </c>
       <c r="G3">
-        <v>1.303792821776162</v>
+        <v>1.227518074963115</v>
       </c>
       <c r="H3">
-        <v>1.303792821776162</v>
+        <v>1.227518074963115</v>
       </c>
       <c r="I3">
-        <v>1.303792821776162</v>
+        <v>1.227518074963115</v>
       </c>
       <c r="J3">
-        <v>1.303792821776162</v>
+        <v>1.227518074963115</v>
       </c>
       <c r="K3">
-        <v>1.303792821776162</v>
+        <v>1.227518074963115</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -899,34 +899,34 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>0.6962071782238374</v>
+        <v>0.7724819250368852</v>
       </c>
       <c r="C4">
-        <v>0.6962071782238374</v>
+        <v>0.7724819250368852</v>
       </c>
       <c r="D4">
-        <v>0.6962071782238374</v>
+        <v>0.7724819250368852</v>
       </c>
       <c r="E4">
-        <v>0.6962071782238374</v>
+        <v>0.7724819250368852</v>
       </c>
       <c r="F4">
-        <v>0.6962071782238374</v>
+        <v>0.7724819250368852</v>
       </c>
       <c r="G4">
-        <v>0.6962071782238374</v>
+        <v>0.7724819250368852</v>
       </c>
       <c r="H4">
-        <v>0.6962071782238374</v>
+        <v>0.7724819250368852</v>
       </c>
       <c r="I4">
-        <v>0.6962071782238374</v>
+        <v>0.7724819250368852</v>
       </c>
       <c r="J4">
-        <v>0.6962071782238374</v>
+        <v>0.7724819250368852</v>
       </c>
       <c r="K4">
-        <v>0.6962071782238374</v>
+        <v>0.7724819250368852</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -934,34 +934,34 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>1.293997060646935</v>
+        <v>1.183204057379025</v>
       </c>
       <c r="C5">
-        <v>1.293997060646935</v>
+        <v>1.183204057379025</v>
       </c>
       <c r="D5">
-        <v>1.293997060646935</v>
+        <v>1.183204057379025</v>
       </c>
       <c r="E5">
-        <v>1.293997060646935</v>
+        <v>1.183204057379025</v>
       </c>
       <c r="F5">
-        <v>1.293997060646935</v>
+        <v>1.183204057379025</v>
       </c>
       <c r="G5">
-        <v>1.293997060646935</v>
+        <v>1.183204057379025</v>
       </c>
       <c r="H5">
-        <v>1.293997060646935</v>
+        <v>1.183204057379025</v>
       </c>
       <c r="I5">
-        <v>1.293997060646935</v>
+        <v>1.183204057379025</v>
       </c>
       <c r="J5">
-        <v>1.293997060646935</v>
+        <v>1.183204057379025</v>
       </c>
       <c r="K5">
-        <v>1.293997060646935</v>
+        <v>1.183204057379025</v>
       </c>
     </row>
   </sheetData>
@@ -987,7 +987,7 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>0.2426304458088387</v>
+        <v>0.2023576762861144</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -995,7 +995,7 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>0.2573695541911614</v>
+        <v>0.2976423237138854</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1003,7 +1003,7 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>0.2573695541911612</v>
+        <v>0.2976423237138855</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1011,7 +1011,7 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>0.2426304458088387</v>
+        <v>0.2023576762861146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add wool to price variation
</commit_message>
<xml_diff>
--- a/PriceScenarios.xlsx
+++ b/PriceScenarios.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="18">
   <si>
     <t>typ</t>
   </si>
@@ -59,6 +59,18 @@
   </si>
   <si>
     <t>c1_3</t>
+  </si>
+  <si>
+    <t>c1_4</t>
+  </si>
+  <si>
+    <t>c1_5</t>
+  </si>
+  <si>
+    <t>c1_6</t>
+  </si>
+  <si>
+    <t>c1_7</t>
   </si>
 </sst>
 </file>
@@ -416,7 +428,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -459,34 +471,34 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>0.9001469258456177</v>
+        <v>0.8917796022511414</v>
       </c>
       <c r="C2">
-        <v>0.9001469258456177</v>
+        <v>0.8917796022511414</v>
       </c>
       <c r="D2">
-        <v>0.9001469258456177</v>
+        <v>0.8917796022511414</v>
       </c>
       <c r="E2">
-        <v>0.9001469258456177</v>
+        <v>0.8917796022511414</v>
       </c>
       <c r="F2">
-        <v>0.9001469258456177</v>
+        <v>0.8917796022511414</v>
       </c>
       <c r="G2">
-        <v>0.9001469258456177</v>
+        <v>0.8917796022511414</v>
       </c>
       <c r="H2">
-        <v>0.9001469258456177</v>
+        <v>0.8917796022511414</v>
       </c>
       <c r="I2">
-        <v>0.9001469258456177</v>
+        <v>0.8917796022511414</v>
       </c>
       <c r="J2">
-        <v>0.9001469258456177</v>
+        <v>0.8917796022511414</v>
       </c>
       <c r="K2">
-        <v>0.9001469258456177</v>
+        <v>0.8917796022511414</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -494,34 +506,34 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>0.8759941262449619</v>
+        <v>0.9097077561761636</v>
       </c>
       <c r="C3">
-        <v>0.8759941262449619</v>
+        <v>0.9097077561761636</v>
       </c>
       <c r="D3">
-        <v>0.8759941262449619</v>
+        <v>0.9097077561761636</v>
       </c>
       <c r="E3">
-        <v>0.8759941262449619</v>
+        <v>0.9097077561761636</v>
       </c>
       <c r="F3">
-        <v>0.8759941262449619</v>
+        <v>0.9097077561761636</v>
       </c>
       <c r="G3">
-        <v>0.8759941262449619</v>
+        <v>0.9097077561761636</v>
       </c>
       <c r="H3">
-        <v>0.8759941262449619</v>
+        <v>0.9097077561761636</v>
       </c>
       <c r="I3">
-        <v>0.8759941262449619</v>
+        <v>0.9097077561761636</v>
       </c>
       <c r="J3">
-        <v>0.8759941262449619</v>
+        <v>0.9097077561761636</v>
       </c>
       <c r="K3">
-        <v>0.8759941262449619</v>
+        <v>0.9097077561761636</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -529,34 +541,34 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>1.124005873755038</v>
+        <v>0.862806697296832</v>
       </c>
       <c r="C4">
-        <v>1.124005873755038</v>
+        <v>0.862806697296832</v>
       </c>
       <c r="D4">
-        <v>1.124005873755038</v>
+        <v>0.862806697296832</v>
       </c>
       <c r="E4">
-        <v>1.124005873755038</v>
+        <v>0.862806697296832</v>
       </c>
       <c r="F4">
-        <v>1.124005873755038</v>
+        <v>0.862806697296832</v>
       </c>
       <c r="G4">
-        <v>1.124005873755038</v>
+        <v>0.862806697296832</v>
       </c>
       <c r="H4">
-        <v>1.124005873755038</v>
+        <v>0.862806697296832</v>
       </c>
       <c r="I4">
-        <v>1.124005873755038</v>
+        <v>0.862806697296832</v>
       </c>
       <c r="J4">
-        <v>1.124005873755038</v>
+        <v>0.862806697296832</v>
       </c>
       <c r="K4">
-        <v>1.124005873755038</v>
+        <v>0.862806697296832</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -564,34 +576,174 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>1.099853074154382</v>
+        <v>0.885528406419913</v>
       </c>
       <c r="C5">
-        <v>1.099853074154382</v>
+        <v>0.885528406419913</v>
       </c>
       <c r="D5">
-        <v>1.099853074154382</v>
+        <v>0.885528406419913</v>
       </c>
       <c r="E5">
-        <v>1.099853074154382</v>
+        <v>0.885528406419913</v>
       </c>
       <c r="F5">
-        <v>1.099853074154382</v>
+        <v>0.885528406419913</v>
       </c>
       <c r="G5">
-        <v>1.099853074154382</v>
+        <v>0.885528406419913</v>
       </c>
       <c r="H5">
-        <v>1.099853074154382</v>
+        <v>0.885528406419913</v>
       </c>
       <c r="I5">
-        <v>1.099853074154382</v>
+        <v>0.885528406419913</v>
       </c>
       <c r="J5">
-        <v>1.099853074154382</v>
+        <v>0.885528406419913</v>
       </c>
       <c r="K5">
-        <v>1.099853074154382</v>
+        <v>0.885528406419913</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>1.114471593580087</v>
+      </c>
+      <c r="C6">
+        <v>1.114471593580087</v>
+      </c>
+      <c r="D6">
+        <v>1.114471593580087</v>
+      </c>
+      <c r="E6">
+        <v>1.114471593580087</v>
+      </c>
+      <c r="F6">
+        <v>1.114471593580087</v>
+      </c>
+      <c r="G6">
+        <v>1.114471593580087</v>
+      </c>
+      <c r="H6">
+        <v>1.114471593580087</v>
+      </c>
+      <c r="I6">
+        <v>1.114471593580087</v>
+      </c>
+      <c r="J6">
+        <v>1.114471593580087</v>
+      </c>
+      <c r="K6">
+        <v>1.114471593580087</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>1.137193302703168</v>
+      </c>
+      <c r="C7">
+        <v>1.137193302703168</v>
+      </c>
+      <c r="D7">
+        <v>1.137193302703168</v>
+      </c>
+      <c r="E7">
+        <v>1.137193302703168</v>
+      </c>
+      <c r="F7">
+        <v>1.137193302703168</v>
+      </c>
+      <c r="G7">
+        <v>1.137193302703168</v>
+      </c>
+      <c r="H7">
+        <v>1.137193302703168</v>
+      </c>
+      <c r="I7">
+        <v>1.137193302703168</v>
+      </c>
+      <c r="J7">
+        <v>1.137193302703168</v>
+      </c>
+      <c r="K7">
+        <v>1.137193302703168</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>1.090292243823836</v>
+      </c>
+      <c r="C8">
+        <v>1.090292243823836</v>
+      </c>
+      <c r="D8">
+        <v>1.090292243823836</v>
+      </c>
+      <c r="E8">
+        <v>1.090292243823836</v>
+      </c>
+      <c r="F8">
+        <v>1.090292243823836</v>
+      </c>
+      <c r="G8">
+        <v>1.090292243823836</v>
+      </c>
+      <c r="H8">
+        <v>1.090292243823836</v>
+      </c>
+      <c r="I8">
+        <v>1.090292243823836</v>
+      </c>
+      <c r="J8">
+        <v>1.090292243823836</v>
+      </c>
+      <c r="K8">
+        <v>1.090292243823836</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>1.108220397748859</v>
+      </c>
+      <c r="C9">
+        <v>1.108220397748859</v>
+      </c>
+      <c r="D9">
+        <v>1.108220397748859</v>
+      </c>
+      <c r="E9">
+        <v>1.108220397748859</v>
+      </c>
+      <c r="F9">
+        <v>1.108220397748859</v>
+      </c>
+      <c r="G9">
+        <v>1.108220397748859</v>
+      </c>
+      <c r="H9">
+        <v>1.108220397748859</v>
+      </c>
+      <c r="I9">
+        <v>1.108220397748859</v>
+      </c>
+      <c r="J9">
+        <v>1.108220397748859</v>
+      </c>
+      <c r="K9">
+        <v>1.108220397748859</v>
       </c>
     </row>
   </sheetData>
@@ -601,7 +753,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -644,34 +796,34 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>0.8167959426209745</v>
+        <v>0.8040309623267345</v>
       </c>
       <c r="C2">
-        <v>0.8167959426209745</v>
+        <v>0.8040309623267345</v>
       </c>
       <c r="D2">
-        <v>0.8167959426209745</v>
+        <v>0.8040309623267345</v>
       </c>
       <c r="E2">
-        <v>0.8167959426209745</v>
+        <v>0.8040309623267345</v>
       </c>
       <c r="F2">
-        <v>0.8167959426209745</v>
+        <v>0.8040309623267345</v>
       </c>
       <c r="G2">
-        <v>0.8167959426209745</v>
+        <v>0.8040309623267345</v>
       </c>
       <c r="H2">
-        <v>0.8167959426209745</v>
+        <v>0.8040309623267345</v>
       </c>
       <c r="I2">
-        <v>0.8167959426209745</v>
+        <v>0.8040309623267345</v>
       </c>
       <c r="J2">
-        <v>0.8167959426209745</v>
+        <v>0.8040309623267345</v>
       </c>
       <c r="K2">
-        <v>0.8167959426209745</v>
+        <v>0.8040309623267345</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -679,34 +831,34 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>1.227518074963115</v>
+        <v>0.8301305515595439</v>
       </c>
       <c r="C3">
-        <v>1.227518074963115</v>
+        <v>0.8301305515595439</v>
       </c>
       <c r="D3">
-        <v>1.227518074963115</v>
+        <v>0.8301305515595439</v>
       </c>
       <c r="E3">
-        <v>1.227518074963115</v>
+        <v>0.8301305515595439</v>
       </c>
       <c r="F3">
-        <v>1.227518074963115</v>
+        <v>0.8301305515595439</v>
       </c>
       <c r="G3">
-        <v>1.227518074963115</v>
+        <v>0.8301305515595439</v>
       </c>
       <c r="H3">
-        <v>1.227518074963115</v>
+        <v>0.8301305515595439</v>
       </c>
       <c r="I3">
-        <v>1.227518074963115</v>
+        <v>0.8301305515595439</v>
       </c>
       <c r="J3">
-        <v>1.227518074963115</v>
+        <v>0.8301305515595439</v>
       </c>
       <c r="K3">
-        <v>1.227518074963115</v>
+        <v>0.8301305515595439</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -714,34 +866,34 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>0.7724819250368852</v>
+        <v>1.215804309908924</v>
       </c>
       <c r="C4">
-        <v>0.7724819250368852</v>
+        <v>1.215804309908924</v>
       </c>
       <c r="D4">
-        <v>0.7724819250368852</v>
+        <v>1.215804309908924</v>
       </c>
       <c r="E4">
-        <v>0.7724819250368852</v>
+        <v>1.215804309908924</v>
       </c>
       <c r="F4">
-        <v>0.7724819250368852</v>
+        <v>1.215804309908924</v>
       </c>
       <c r="G4">
-        <v>0.7724819250368852</v>
+        <v>1.215804309908924</v>
       </c>
       <c r="H4">
-        <v>0.7724819250368852</v>
+        <v>1.215804309908924</v>
       </c>
       <c r="I4">
-        <v>0.7724819250368852</v>
+        <v>1.215804309908924</v>
       </c>
       <c r="J4">
-        <v>0.7724819250368852</v>
+        <v>1.215804309908924</v>
       </c>
       <c r="K4">
-        <v>0.7724819250368852</v>
+        <v>1.215804309908924</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -749,34 +901,174 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>1.183204057379025</v>
+        <v>1.248158231333236</v>
       </c>
       <c r="C5">
-        <v>1.183204057379025</v>
+        <v>1.248158231333236</v>
       </c>
       <c r="D5">
-        <v>1.183204057379025</v>
+        <v>1.248158231333236</v>
       </c>
       <c r="E5">
-        <v>1.183204057379025</v>
+        <v>1.248158231333236</v>
       </c>
       <c r="F5">
-        <v>1.183204057379025</v>
+        <v>1.248158231333236</v>
       </c>
       <c r="G5">
-        <v>1.183204057379025</v>
+        <v>1.248158231333236</v>
       </c>
       <c r="H5">
-        <v>1.183204057379025</v>
+        <v>1.248158231333236</v>
       </c>
       <c r="I5">
-        <v>1.183204057379025</v>
+        <v>1.248158231333236</v>
       </c>
       <c r="J5">
-        <v>1.183204057379025</v>
+        <v>1.248158231333236</v>
       </c>
       <c r="K5">
-        <v>1.183204057379025</v>
+        <v>1.248158231333236</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>0.7518417686667644</v>
+      </c>
+      <c r="C6">
+        <v>0.7518417686667644</v>
+      </c>
+      <c r="D6">
+        <v>0.7518417686667644</v>
+      </c>
+      <c r="E6">
+        <v>0.7518417686667644</v>
+      </c>
+      <c r="F6">
+        <v>0.7518417686667644</v>
+      </c>
+      <c r="G6">
+        <v>0.7518417686667644</v>
+      </c>
+      <c r="H6">
+        <v>0.7518417686667644</v>
+      </c>
+      <c r="I6">
+        <v>0.7518417686667644</v>
+      </c>
+      <c r="J6">
+        <v>0.7518417686667644</v>
+      </c>
+      <c r="K6">
+        <v>0.7518417686667644</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>0.784195690091076</v>
+      </c>
+      <c r="C7">
+        <v>0.784195690091076</v>
+      </c>
+      <c r="D7">
+        <v>0.784195690091076</v>
+      </c>
+      <c r="E7">
+        <v>0.784195690091076</v>
+      </c>
+      <c r="F7">
+        <v>0.784195690091076</v>
+      </c>
+      <c r="G7">
+        <v>0.784195690091076</v>
+      </c>
+      <c r="H7">
+        <v>0.784195690091076</v>
+      </c>
+      <c r="I7">
+        <v>0.784195690091076</v>
+      </c>
+      <c r="J7">
+        <v>0.784195690091076</v>
+      </c>
+      <c r="K7">
+        <v>0.784195690091076</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>1.169869448440456</v>
+      </c>
+      <c r="C8">
+        <v>1.169869448440456</v>
+      </c>
+      <c r="D8">
+        <v>1.169869448440456</v>
+      </c>
+      <c r="E8">
+        <v>1.169869448440456</v>
+      </c>
+      <c r="F8">
+        <v>1.169869448440456</v>
+      </c>
+      <c r="G8">
+        <v>1.169869448440456</v>
+      </c>
+      <c r="H8">
+        <v>1.169869448440456</v>
+      </c>
+      <c r="I8">
+        <v>1.169869448440456</v>
+      </c>
+      <c r="J8">
+        <v>1.169869448440456</v>
+      </c>
+      <c r="K8">
+        <v>1.169869448440456</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>1.195969037673266</v>
+      </c>
+      <c r="C9">
+        <v>1.195969037673266</v>
+      </c>
+      <c r="D9">
+        <v>1.195969037673266</v>
+      </c>
+      <c r="E9">
+        <v>1.195969037673266</v>
+      </c>
+      <c r="F9">
+        <v>1.195969037673266</v>
+      </c>
+      <c r="G9">
+        <v>1.195969037673266</v>
+      </c>
+      <c r="H9">
+        <v>1.195969037673266</v>
+      </c>
+      <c r="I9">
+        <v>1.195969037673266</v>
+      </c>
+      <c r="J9">
+        <v>1.195969037673266</v>
+      </c>
+      <c r="K9">
+        <v>1.195969037673266</v>
       </c>
     </row>
   </sheetData>
@@ -786,7 +1078,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -829,34 +1121,34 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>0.8167959426209745</v>
+        <v>0.9093036898722159</v>
       </c>
       <c r="C2">
-        <v>0.8167959426209745</v>
+        <v>0.9093036898722159</v>
       </c>
       <c r="D2">
-        <v>0.8167959426209745</v>
+        <v>0.9093036898722159</v>
       </c>
       <c r="E2">
-        <v>0.8167959426209745</v>
+        <v>0.9093036898722159</v>
       </c>
       <c r="F2">
-        <v>0.8167959426209745</v>
+        <v>0.9093036898722159</v>
       </c>
       <c r="G2">
-        <v>0.8167959426209745</v>
+        <v>0.9093036898722159</v>
       </c>
       <c r="H2">
-        <v>0.8167959426209745</v>
+        <v>0.9093036898722159</v>
       </c>
       <c r="I2">
-        <v>0.8167959426209745</v>
+        <v>0.9093036898722159</v>
       </c>
       <c r="J2">
-        <v>0.8167959426209745</v>
+        <v>0.9093036898722159</v>
       </c>
       <c r="K2">
-        <v>0.8167959426209745</v>
+        <v>0.9093036898722159</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -864,34 +1156,34 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>1.227518074963115</v>
+        <v>1.065598434559732</v>
       </c>
       <c r="C3">
-        <v>1.227518074963115</v>
+        <v>1.065598434559732</v>
       </c>
       <c r="D3">
-        <v>1.227518074963115</v>
+        <v>1.065598434559732</v>
       </c>
       <c r="E3">
-        <v>1.227518074963115</v>
+        <v>1.065598434559732</v>
       </c>
       <c r="F3">
-        <v>1.227518074963115</v>
+        <v>1.065598434559732</v>
       </c>
       <c r="G3">
-        <v>1.227518074963115</v>
+        <v>1.065598434559732</v>
       </c>
       <c r="H3">
-        <v>1.227518074963115</v>
+        <v>1.065598434559732</v>
       </c>
       <c r="I3">
-        <v>1.227518074963115</v>
+        <v>1.065598434559732</v>
       </c>
       <c r="J3">
-        <v>1.227518074963115</v>
+        <v>1.065598434559732</v>
       </c>
       <c r="K3">
-        <v>1.227518074963115</v>
+        <v>1.065598434559732</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -899,34 +1191,34 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>0.7724819250368852</v>
+        <v>0.921135610673716</v>
       </c>
       <c r="C4">
-        <v>0.7724819250368852</v>
+        <v>0.921135610673716</v>
       </c>
       <c r="D4">
-        <v>0.7724819250368852</v>
+        <v>0.921135610673716</v>
       </c>
       <c r="E4">
-        <v>0.7724819250368852</v>
+        <v>0.921135610673716</v>
       </c>
       <c r="F4">
-        <v>0.7724819250368852</v>
+        <v>0.921135610673716</v>
       </c>
       <c r="G4">
-        <v>0.7724819250368852</v>
+        <v>0.921135610673716</v>
       </c>
       <c r="H4">
-        <v>0.7724819250368852</v>
+        <v>0.921135610673716</v>
       </c>
       <c r="I4">
-        <v>0.7724819250368852</v>
+        <v>0.921135610673716</v>
       </c>
       <c r="J4">
-        <v>0.7724819250368852</v>
+        <v>0.921135610673716</v>
       </c>
       <c r="K4">
-        <v>0.7724819250368852</v>
+        <v>0.921135610673716</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -934,34 +1226,174 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>1.183204057379025</v>
+        <v>1.075750587078096</v>
       </c>
       <c r="C5">
-        <v>1.183204057379025</v>
+        <v>1.075750587078096</v>
       </c>
       <c r="D5">
-        <v>1.183204057379025</v>
+        <v>1.075750587078096</v>
       </c>
       <c r="E5">
-        <v>1.183204057379025</v>
+        <v>1.075750587078096</v>
       </c>
       <c r="F5">
-        <v>1.183204057379025</v>
+        <v>1.075750587078096</v>
       </c>
       <c r="G5">
-        <v>1.183204057379025</v>
+        <v>1.075750587078096</v>
       </c>
       <c r="H5">
-        <v>1.183204057379025</v>
+        <v>1.075750587078096</v>
       </c>
       <c r="I5">
-        <v>1.183204057379025</v>
+        <v>1.075750587078096</v>
       </c>
       <c r="J5">
-        <v>1.183204057379025</v>
+        <v>1.075750587078096</v>
       </c>
       <c r="K5">
-        <v>1.183204057379025</v>
+        <v>1.075750587078096</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>0.9242494129219041</v>
+      </c>
+      <c r="C6">
+        <v>0.9242494129219041</v>
+      </c>
+      <c r="D6">
+        <v>0.9242494129219041</v>
+      </c>
+      <c r="E6">
+        <v>0.9242494129219041</v>
+      </c>
+      <c r="F6">
+        <v>0.9242494129219041</v>
+      </c>
+      <c r="G6">
+        <v>0.9242494129219041</v>
+      </c>
+      <c r="H6">
+        <v>0.9242494129219041</v>
+      </c>
+      <c r="I6">
+        <v>0.9242494129219041</v>
+      </c>
+      <c r="J6">
+        <v>0.9242494129219041</v>
+      </c>
+      <c r="K6">
+        <v>0.9242494129219041</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>1.078864389326284</v>
+      </c>
+      <c r="C7">
+        <v>1.078864389326284</v>
+      </c>
+      <c r="D7">
+        <v>1.078864389326284</v>
+      </c>
+      <c r="E7">
+        <v>1.078864389326284</v>
+      </c>
+      <c r="F7">
+        <v>1.078864389326284</v>
+      </c>
+      <c r="G7">
+        <v>1.078864389326284</v>
+      </c>
+      <c r="H7">
+        <v>1.078864389326284</v>
+      </c>
+      <c r="I7">
+        <v>1.078864389326284</v>
+      </c>
+      <c r="J7">
+        <v>1.078864389326284</v>
+      </c>
+      <c r="K7">
+        <v>1.078864389326284</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>0.9344015654402679</v>
+      </c>
+      <c r="C8">
+        <v>0.9344015654402679</v>
+      </c>
+      <c r="D8">
+        <v>0.9344015654402679</v>
+      </c>
+      <c r="E8">
+        <v>0.9344015654402679</v>
+      </c>
+      <c r="F8">
+        <v>0.9344015654402679</v>
+      </c>
+      <c r="G8">
+        <v>0.9344015654402679</v>
+      </c>
+      <c r="H8">
+        <v>0.9344015654402679</v>
+      </c>
+      <c r="I8">
+        <v>0.9344015654402679</v>
+      </c>
+      <c r="J8">
+        <v>0.9344015654402679</v>
+      </c>
+      <c r="K8">
+        <v>0.9344015654402679</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>1.090696310127785</v>
+      </c>
+      <c r="C9">
+        <v>1.090696310127785</v>
+      </c>
+      <c r="D9">
+        <v>1.090696310127785</v>
+      </c>
+      <c r="E9">
+        <v>1.090696310127785</v>
+      </c>
+      <c r="F9">
+        <v>1.090696310127785</v>
+      </c>
+      <c r="G9">
+        <v>1.090696310127785</v>
+      </c>
+      <c r="H9">
+        <v>1.090696310127785</v>
+      </c>
+      <c r="I9">
+        <v>1.090696310127785</v>
+      </c>
+      <c r="J9">
+        <v>1.090696310127785</v>
+      </c>
+      <c r="K9">
+        <v>1.090696310127785</v>
       </c>
     </row>
   </sheetData>
@@ -971,7 +1403,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -987,7 +1419,7 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>0.2023576762861144</v>
+        <v>0.1300397501860382</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -995,7 +1427,7 @@
         <v>11</v>
       </c>
       <c r="B3">
-        <v>0.2976423237138854</v>
+        <v>0.07264965140027922</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1003,7 +1435,7 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>0.2976423237138855</v>
+        <v>0.1539326632094</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1011,7 +1443,39 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>0.2023576762861146</v>
+        <v>0.1433779352042823</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>0.1433779352042824</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>0.1539326632094002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>0.07264965140027926</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>0.1300397501860383</v>
       </c>
     </row>
   </sheetData>

</xml_diff>